<commit_message>
Modify some smoke script to make them stable to handle the delay time.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TST2806_VerifySiteIdUsedInRunCommandAction.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TST2806_VerifySiteIdUsedInRunCommandAction.xlsx
@@ -1209,7 +1209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7517" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7526" uniqueCount="849">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3604,183 +3604,179 @@
     <t>T</t>
   </si>
   <si>
+    <t>"testuser"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>;Add some devices.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pause</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Click</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Click</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Text</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testpublic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"public"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormManaged_Devices</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{CONTROL down}{Akey}{CONTROL up}"</t>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"nform testing"</t>
+  </si>
+  <si>
+    <t>"2"</t>
+  </si>
+  <si>
+    <t>"Run-command"</t>
+  </si>
+  <si>
+    <t>"C:\Nform\result2.dat"</t>
+  </si>
+  <si>
+    <t>;should be reflected in 'Device Properties' dialog box say in SNMP and Communication tab.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;The goal of this test is to configure and test a Set Action is to generate traps when related action set is under action.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">;Prerequisites 1. NformG2 software installed on windows operating System. 2. Advanced communication license must be added before adding devices. 3. User should have permission to 'Write Data Action' under Groups. 4. SNMP devices should be added before going for test action. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$GXT_0$</t>
+  </si>
+  <si>
+    <t>Update Date</t>
+  </si>
+  <si>
     <t>T</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"testuser"</t>
+    <t>62</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Running Range</t>
+  </si>
+  <si>
+    <t>FormManaged_Devices</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>;Add some devices.</t>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>FormAdd_Device</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>$SNMPdevice_0$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>"ABC GXT UPS 100"</t>
+  </si>
+  <si>
+    <t>"Description for GXT"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Liebert GXT UPS/WebCard"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"SNMP"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormAdd_Device_Results</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Close</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Pause</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Script Info</t>
+  </si>
+  <si>
+    <t>Script Data</t>
+  </si>
+  <si>
+    <t>Test Object</t>
+  </si>
+  <si>
+    <t>C:\\Nform\\bin\\NformViewer.exe</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Create Date</t>
   </si>
   <si>
     <t>Click</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Click</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Checked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Text</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>testpublic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"public"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>FormManaged_Devices</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>"{CONTROL down}{Akey}{CONTROL up}"</t>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"nform testing"</t>
-  </si>
-  <si>
-    <t>"2"</t>
-  </si>
-  <si>
-    <t>"Run-command"</t>
-  </si>
-  <si>
-    <t>"C:\Nform\result2.dat"</t>
-  </si>
-  <si>
-    <t>;should be reflected in 'Device Properties' dialog box say in SNMP and Communication tab.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>;The goal of this test is to configure and test a Set Action is to generate traps when related action set is under action.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">;Prerequisites 1. NformG2 software installed on windows operating System. 2. Advanced communication license must be added before adding devices. 3. User should have permission to 'Write Data Action' under Groups. 4. SNMP devices should be added before going for test action. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$GXT_0$</t>
-  </si>
-  <si>
-    <t>Update Date</t>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>62</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Running Range</t>
-  </si>
-  <si>
-    <t>FormManaged_Devices</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>FormAdd_Device</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>$SNMPdevice_0$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"ABC GXT UPS 100"</t>
-  </si>
-  <si>
-    <t>"Description for GXT"</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Liebert GXT UPS/WebCard"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"SNMP"</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>FormAdd_Device_Results</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Close</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pause</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Script Info</t>
-  </si>
-  <si>
-    <t>Script Data</t>
-  </si>
-  <si>
-    <t>Test Object</t>
-  </si>
-  <si>
-    <t>C:\\Nform\\bin\\NformViewer.exe</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>Create Date</t>
-  </si>
-  <si>
-    <t>Click</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"nform testing"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3797,15 +3793,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>25-42</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"action-runcommand"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>;Create Run-command Action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>82</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4042,35 +4046,7 @@
     <cellStyle name="常规 2 2" xfId="3"/>
     <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -4823,10 +4799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4843,10 +4819,10 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>831</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>832</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>757</v>
@@ -4888,10 +4864,10 @@
     </row>
     <row r="2" spans="1:15" ht="15">
       <c r="A2" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>833</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>834</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -4913,10 +4889,10 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>835</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>836</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
@@ -4948,10 +4924,10 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>837</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>838</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -4979,7 +4955,7 @@
     </row>
     <row r="5" spans="1:15" ht="15">
       <c r="A5" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B5" s="10">
         <v>41106</v>
@@ -4988,7 +4964,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -5004,7 +4980,7 @@
     </row>
     <row r="6" spans="1:15" ht="15">
       <c r="A6" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B6" s="10">
         <v>41106</v>
@@ -5013,7 +4989,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -5032,13 +5008,13 @@
         <v>765</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>817</v>
+        <v>848</v>
       </c>
       <c r="C7" s="5">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -5054,16 +5030,14 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
-        <v>818</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>845</v>
-      </c>
+        <v>817</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="5">
         <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>19</v>
@@ -5085,14 +5059,14 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="5">
         <v>8</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>19</v>
@@ -5123,10 +5097,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>183</v>
@@ -5150,10 +5124,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>166</v>
@@ -5179,10 +5153,10 @@
         <v>11</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>381</v>
@@ -5191,7 +5165,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="5"/>
@@ -5210,10 +5184,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>607</v>
@@ -5239,10 +5213,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>166</v>
@@ -5295,10 +5269,10 @@
         <v>15</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>256</v>
@@ -5307,7 +5281,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="5"/>
@@ -5326,10 +5300,10 @@
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>255</v>
@@ -5338,7 +5312,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="5"/>
@@ -5357,10 +5331,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>519</v>
@@ -5369,7 +5343,7 @@
         <v>13</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -5388,10 +5362,10 @@
         <v>18</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>608</v>
@@ -5400,7 +5374,7 @@
         <v>13</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -5421,10 +5395,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>603</v>
@@ -5477,10 +5451,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>17</v>
@@ -5504,13 +5478,13 @@
         <v>22</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>2</v>
@@ -5531,10 +5505,10 @@
         <v>23</v>
       </c>
       <c r="D24" s="21" t="s">
+        <v>828</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>829</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>830</v>
       </c>
       <c r="F24" s="11">
         <v>5</v>
@@ -5554,7 +5528,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="5"/>
@@ -5573,7 +5547,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>19</v>
@@ -5598,7 +5572,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>19</v>
@@ -5623,7 +5597,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>306</v>
@@ -5648,7 +5622,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>310</v>
@@ -5660,7 +5634,7 @@
         <v>4</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -5675,7 +5649,7 @@
         <v>29</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>310</v>
@@ -5687,7 +5661,7 @@
         <v>4</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -5702,7 +5676,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>310</v>
@@ -5736,7 +5710,7 @@
         <v>283</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
@@ -5761,7 +5735,7 @@
         <v>17</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H33" s="11"/>
       <c r="I33" s="5"/>
@@ -5789,7 +5763,7 @@
         <v>4</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I34" s="11"/>
       <c r="J34" s="5"/>
@@ -5816,7 +5790,7 @@
         <v>4</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I35" s="11"/>
       <c r="J35" s="5"/>
@@ -5843,7 +5817,7 @@
         <v>3</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I36" s="11"/>
       <c r="J36" s="5"/>
@@ -5870,7 +5844,7 @@
         <v>3</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="I37" s="11"/>
       <c r="J37" s="5"/>
@@ -5897,7 +5871,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="5"/>
@@ -5960,7 +5934,7 @@
         <v>40</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>310</v>
@@ -5985,7 +5959,7 @@
         <v>41</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>306</v>
@@ -6033,7 +6007,7 @@
         <v>43</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="5"/>
@@ -6114,7 +6088,7 @@
         <v>56</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
@@ -6129,17 +6103,15 @@
         <v>47</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>785</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>2</v>
-      </c>
+        <v>756</v>
+      </c>
+      <c r="F48" s="5">
+        <v>5</v>
+      </c>
+      <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
@@ -6149,18 +6121,24 @@
       <c r="N48" s="7"/>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" spans="3:15" ht="15">
+    <row r="49" spans="3:15">
       <c r="C49" s="5">
         <v>48</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>786</v>
-      </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
+      <c r="D49" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>785</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
@@ -6173,13 +6151,13 @@
         <v>49</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>792</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>19</v>
+        <v>784</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>518</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>2</v>
@@ -6190,20 +6168,21 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
-      <c r="N50" s="16"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="2"/>
     </row>
     <row r="51" spans="3:15">
       <c r="C51" s="5">
         <v>50</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>792</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>19</v>
+        <v>784</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>785</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>2</v>
@@ -6214,51 +6193,45 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
-      <c r="N51" s="16"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="2"/>
     </row>
-    <row r="52" spans="3:15">
+    <row r="52" spans="3:15" ht="15">
       <c r="C52" s="5">
         <v>51</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>792</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>793</v>
-      </c>
-      <c r="I52" s="5"/>
+      <c r="D52" s="6" t="s">
+        <v>786</v>
+      </c>
+      <c r="E52" s="11"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
-      <c r="N52" s="16"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="2"/>
     </row>
     <row r="53" spans="3:15">
       <c r="C53" s="5">
         <v>52</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>792</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>241</v>
+        <v>846</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>245</v>
+        <v>22</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H53" s="11"/>
+      <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
@@ -6271,19 +6244,19 @@
         <v>53</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>791</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>241</v>
+        <v>846</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -6295,17 +6268,21 @@
         <v>54</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>796</v>
+        <v>846</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>795</v>
-      </c>
-      <c r="F55" s="5">
-        <v>2</v>
-      </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
+        <v>241</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -6317,74 +6294,70 @@
         <v>55</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>784</v>
+        <v>846</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>22</v>
+        <v>245</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>797</v>
-      </c>
-      <c r="H56" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="H56" s="11"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
-      <c r="N56" s="7"/>
+      <c r="N56" s="16"/>
     </row>
     <row r="57" spans="3:15">
       <c r="C57" s="5">
         <v>56</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>784</v>
+        <v>847</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>797</v>
-      </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="2"/>
+      <c r="N57" s="16"/>
     </row>
     <row r="58" spans="3:15">
       <c r="C58" s="5">
         <v>57</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>784</v>
+        <v>795</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>797</v>
-      </c>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
+        <v>794</v>
+      </c>
+      <c r="F58" s="5">
+        <v>2</v>
+      </c>
+      <c r="G58" s="5"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="2"/>
+      <c r="N58" s="16"/>
     </row>
     <row r="59" spans="3:15">
       <c r="C59" s="5">
@@ -6394,28 +6367,21 @@
         <v>784</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>396</v>
+        <v>19</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>360</v>
+        <v>22</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>790</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="J59" s="5">
-        <v>1500</v>
-      </c>
+        <v>796</v>
+      </c>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
       <c r="N59" s="7"/>
-      <c r="O59" s="2"/>
     </row>
     <row r="60" spans="3:15">
       <c r="C60" s="5">
@@ -6425,13 +6391,13 @@
         <v>784</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>396</v>
+        <v>19</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>358</v>
+        <v>83</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
@@ -6453,20 +6419,14 @@
         <v>396</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>360</v>
+        <v>401</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>790</v>
-      </c>
-      <c r="I61" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="J61" s="5">
-        <v>1000</v>
-      </c>
+        <v>796</v>
+      </c>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
@@ -6484,7 +6444,7 @@
         <v>396</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>480</v>
+        <v>360</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>7</v>
@@ -6496,7 +6456,7 @@
         <v>788</v>
       </c>
       <c r="J62" s="5">
-        <v>1</v>
+        <v>1500</v>
       </c>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
@@ -6515,10 +6475,10 @@
         <v>396</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>477</v>
+        <v>358</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>2</v>
+        <v>797</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -6540,7 +6500,7 @@
         <v>396</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>480</v>
+        <v>360</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>7</v>
@@ -6552,7 +6512,7 @@
         <v>788</v>
       </c>
       <c r="J64" s="5">
-        <v>2</v>
+        <v>1000</v>
       </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
@@ -6571,18 +6531,20 @@
         <v>396</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>799</v>
-      </c>
-      <c r="I65" s="5" t="b">
+        <v>790</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="J65" s="5">
         <v>1</v>
       </c>
-      <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
@@ -6600,20 +6562,14 @@
         <v>396</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>800</v>
-      </c>
-      <c r="I66" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="J66" s="5">
-        <v>65534</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
       <c r="M66" s="5"/>
@@ -6631,14 +6587,20 @@
         <v>396</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="J67" s="5">
+        <v>2</v>
+      </c>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
       <c r="M67" s="5"/>
@@ -6656,20 +6618,18 @@
         <v>396</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>800</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="J68" s="5">
-        <v>65535</v>
-      </c>
+        <v>798</v>
+      </c>
+      <c r="I68" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J68" s="5"/>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
       <c r="M68" s="5"/>
@@ -6687,14 +6647,20 @@
         <v>396</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="J69" s="5">
+        <v>65534</v>
+      </c>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
       <c r="M69" s="5"/>
@@ -6712,20 +6678,14 @@
         <v>396</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>800</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>801</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
       <c r="M70" s="5"/>
@@ -6743,19 +6703,19 @@
         <v>396</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>382</v>
+        <v>476</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="J71" s="5" t="s">
-        <v>801</v>
+      <c r="J71" s="5">
+        <v>65535</v>
       </c>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
@@ -6774,14 +6734,12 @@
         <v>396</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>802</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
@@ -6801,16 +6759,20 @@
         <v>396</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>382</v>
+        <v>470</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>802</v>
-      </c>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
+        <v>799</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>800</v>
+      </c>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
       <c r="M73" s="5"/>
@@ -6828,14 +6790,20 @@
         <v>396</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>17</v>
+        <v>382</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>800</v>
+      </c>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
       <c r="M74" s="5"/>
@@ -6847,24 +6815,26 @@
         <v>74</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>19</v>
+        <v>396</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>22</v>
+        <v>470</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H75" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>801</v>
+      </c>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
       <c r="M75" s="5"/>
-      <c r="N75" s="16"/>
+      <c r="N75" s="7"/>
       <c r="O75" s="2"/>
     </row>
     <row r="76" spans="3:15">
@@ -6872,93 +6842,96 @@
         <v>75</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>19</v>
+        <v>396</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>78</v>
+        <v>382</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="I76" s="5"/>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
       <c r="M76" s="5"/>
-      <c r="N76" s="16"/>
+      <c r="N76" s="7"/>
+      <c r="O76" s="2"/>
     </row>
     <row r="77" spans="3:15">
       <c r="C77" s="5">
         <v>76</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>803</v>
+        <v>784</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>804</v>
+        <v>396</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>578</v>
+        <v>17</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>842</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>805</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
       <c r="M77" s="5"/>
-      <c r="N77" s="16"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="2"/>
     </row>
-    <row r="78" spans="3:15" ht="14.25">
+    <row r="78" spans="3:15">
       <c r="C78" s="5">
         <v>77</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>803</v>
+        <v>791</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>804</v>
+        <v>19</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>184</v>
+        <v>22</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H78" s="17"/>
+      <c r="H78" s="11"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
       <c r="M78" s="5"/>
       <c r="N78" s="16"/>
+      <c r="O78" s="2"/>
     </row>
     <row r="79" spans="3:15">
       <c r="C79" s="5">
         <v>78</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>803</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>585</v>
+        <v>791</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H79" s="11"/>
-      <c r="I79" s="5"/>
+      <c r="I79" s="11"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
@@ -6970,62 +6943,136 @@
         <v>79</v>
       </c>
       <c r="D80" s="8" t="s">
+        <v>802</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>803</v>
       </c>
-      <c r="E80" s="11" t="s">
+      <c r="F80" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="H80" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="F80" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
+      <c r="I80" s="5"/>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
       <c r="M80" s="5"/>
       <c r="N80" s="16"/>
     </row>
+    <row r="81" spans="3:14" ht="14.25">
+      <c r="C81" s="5">
+        <v>80</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>802</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>803</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H81" s="17"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="16"/>
+    </row>
+    <row r="82" spans="3:14">
+      <c r="C82" s="5">
+        <v>81</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>802</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H82" s="11"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="16"/>
+    </row>
+    <row r="83" spans="3:14">
+      <c r="C83" s="5">
+        <v>82</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>802</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>803</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="16"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="N2:N80">
-    <cfRule type="cellIs" dxfId="7" priority="25" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N2:N83">
+    <cfRule type="cellIs" dxfId="5" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="26" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N75:N80">
-    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N78:N83">
+    <cfRule type="cellIs" dxfId="3" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N75:N80">
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N78:N83">
+    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D50:D55 D75:D76 D3:D4 D8:D24 D26:D31 D33 D41:D42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D53:D58 D78:D79 D3:D4 D8:D24 D26:D31 D33 D41:D42">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G78:G80 G2:G76">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G81:G83 G2:G79">
       <formula1>INDIRECT(SUBSTITUTE(E2&amp;F2," ",""))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F80">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F83">
       <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(E2&amp;"Col")),1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E80">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E83">
       <formula1>Forms</formula1>
     </dataValidation>
   </dataValidations>
@@ -28908,39 +28955,39 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>831</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>833</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>835</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>837</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B5" s="10">
         <v>41106</v>
@@ -28948,7 +28995,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B6" s="10">
         <v>41106</v>
@@ -28959,18 +29006,18 @@
         <v>765</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B9" s="12"/>
     </row>
@@ -29064,7 +29111,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="11" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>